<commit_message>
adding experiment and animal to excel
</commit_message>
<xml_diff>
--- a/MatlabAnalysis/periEventAnalysis.xlsx
+++ b/MatlabAnalysis/periEventAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6684"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="6684" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="working sheet" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
   <si>
     <t>BDA TPA Path</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>experiment</t>
+  </si>
+  <si>
+    <t>M26</t>
+  </si>
+  <si>
+    <t>9_24_17</t>
+  </si>
+  <si>
+    <t>9_28_17</t>
+  </si>
+  <si>
+    <t>10_1_17</t>
   </si>
 </sst>
 </file>
@@ -380,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="A2:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="D2" sqref="D2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +451,7 @@
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +461,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -460,8 +478,14 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -471,8 +495,14 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -481,6 +511,12 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -490,10 +526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D2" sqref="D2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +538,7 @@
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,8 +548,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -523,8 +565,14 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -534,8 +582,14 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -544,6 +598,12 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -553,10 +613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +625,7 @@
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,8 +635,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -586,8 +652,14 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -597,8 +669,14 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -607,6 +685,12 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>